<commit_message>
Update content related to precision oncology therapies page (#1028)
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/precisionOncologyTherapies/precision_oncology_therapies.xlsx
+++ b/src/main/webapp/content/files/precisionOncologyTherapies/precision_oncology_therapies.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangh2/repos/oncokb-public/src/main/webapp/content/files/precisionOncologyTherapies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A5FC92-3B3D-AB4D-B065-0289B1E24785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E94F7CD-69E6-6345-AAD3-86ABA0F4355B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="31680" windowHeight="20200" xr2:uid="{D3CC899A-FE92-8343-9D2C-EF5EE5721116}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="17280" windowHeight="20200" xr2:uid="{D3CC899A-FE92-8343-9D2C-EF5EE5721116}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Precision Oncology Therapies" sheetId="1" r:id="rId1"/>
     <sheet name="Footnotes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="200">
   <si>
     <t>1998 – 2001*</t>
   </si>
@@ -407,9 +407,6 @@
     <t>KIT D816</t>
   </si>
   <si>
-    <t>a The first year the drug received FDA-approval in any indication, irrespective of biomarker</t>
-  </si>
-  <si>
     <t>Year of drug’s first FDA-approval a</t>
   </si>
   <si>
@@ -425,31 +422,12 @@
     <t>b Includes pathogeomonic and indication-specific biomarkers, that while not specifically listed in the Indications and Usage section of the FDA drug label, are targeted by the precision oncology drug (ex KIT D816 in systemic mastocytosis [avapritinib] and SMARCB1 deletion in epithelioid sarcoma [tazemetostat])</t>
   </si>
   <si>
-    <t>c If there is a corresponding FDA-approved companion diagnostic test for biomarker identification, this detection method is listed; if a DNA NGS-based detection method can be used to identify the biomarker, this is noted</t>
-  </si>
-  <si>
-    <t>d Only drugs with an FDA-specified biomarker that can be detected by an NGS-based (DNA) assay are classified</t>
-  </si>
-  <si>
     <t>e Pembrolizumab in combination with lenvatinib is FDA-approved approved for endometrial cancer that is pMMR</t>
   </si>
   <si>
     <t>* The exact year of the drug’s first FDA-approval could not be determined due to absent or ambiguous data on FDA.gov website</t>
   </si>
   <si>
-    <t>NGS, Next-generation sequencing; ER, Estrogen Receptor; HR, Hormone Receptor; MSI-H, Microsatellite instability-high; HRR, Homologous Recombination Repair; TMB-H, Tumor mutational burden-high; dMMR, mismatch repair deficient; pMMR, mismatch repair proficient; PMSA, prostate-specific membrane antigen</t>
-  </si>
-  <si>
-    <t>First-in class = 33; Mechanistically-distinct = 7; Follow-on = 19; Resistance = 10</t>
-  </si>
-  <si>
-    <t>Precision oncology therapy: A drug that is most effective in a molecularly defined subset of patients and for which pre-treatment molecular profiling is required for optimal patient selection
-First-in-class precision oncology therapy: A precision oncology therapy targeting an alteration previously classified as not actionable
-Mechanistically-distinct precision oncology therapy: A precision oncology therapy targeting a previously actionable genomic alteration via a distinct mechanisms-of-action, or with significantly different selectivity versus older drugs
-Follow-on precision oncology therapy: A precision oncology therapy with a mechanism of action largely similar to a previously FDA-approved first-in-class drug
-Resistance precision oncology therapy: A precision oncology therapy with a mechanism of action largely similar to an FDA-approved first-in-class precision oncology drug, but with an expanded mutation profile that targets mutations that arise in the context of resistance to the first-in-class drug</t>
-  </si>
-  <si>
     <t>DNA/NGS-based detection or FISH</t>
   </si>
   <si>
@@ -459,9 +437,6 @@
     <t>EGFR L858R and Exon 19 Deletions</t>
   </si>
   <si>
-    <t>KRAS wildtype, EGFR-expressing</t>
-  </si>
-  <si>
     <t>DNA/NGS-based detection </t>
   </si>
   <si>
@@ -498,9 +473,6 @@
     <t>BRCA1/2 Oncogenic Mutations</t>
   </si>
   <si>
-    <t>HRR Gene Oncogenic Mutations</t>
-  </si>
-  <si>
     <t>PD-L1 Expression</t>
   </si>
   <si>
@@ -555,9 +527,6 @@
     <t>BRAF V600E</t>
   </si>
   <si>
-    <t>FGFR1Fusions</t>
-  </si>
-  <si>
     <t>RET Fusions and Oncogenic Mutations</t>
   </si>
   <si>
@@ -573,9 +542,6 @@
     <t>EGFR Exon 20 Insertions</t>
   </si>
   <si>
-    <t>ABL1 T315I</t>
-  </si>
-  <si>
     <t>VHL Oncogenic Mutations</t>
   </si>
   <si>
@@ -589,13 +555,213 @@
   </si>
   <si>
     <t>DNA/HLA-typing</t>
+  </si>
+  <si>
+    <t>c If there is a corresponding FDA-cleared or -approved companion diagnostic device for biomarker identification, the detection method associated with this device is listed; if the biomarker can be detected by a DNA/NGS-based detection method this is listed first</t>
+  </si>
+  <si>
+    <t>d Only drugs with an FDA-specified biomarker that can be detected by a DNA/NGS-based detection method are classified</t>
+  </si>
+  <si>
+    <t>a The first year the drug received FDA-approval in any indication, irrespective of whether the biomarker was included in the FDA-drug at that time</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Precision oncology therapy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A drug that is most effective in a molecularly defined subset of patients and for which pre-treatment molecular profiling is required for optimal patient selection
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>First-in-class precision oncology therapy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A precision oncology therapy targeting an alteration previously classified as not actionable
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mechanistically-distinct precision oncology therapy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A precision oncology therapy targeting a previously actionable genomic alteration via a distinct mechanisms-of-action, or with significantly different selectivity versus older drugs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Follow-on precision oncology therapy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A precision oncology therapy with a mechanism of action largely similar to a previously FDA-approved first-in-class precision oncology drug
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resistance precision oncology therapy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A precision oncology therapy with a mechanism of action largely similar to an FDA-approved first-in-class precision oncology drug, but with an expanded mutation profile that targets mutations that arise in the context of resistance to the first-in-class drug</t>
+    </r>
+  </si>
+  <si>
+    <t>First-in class = 34; Mechanistically-distinct = 9; Follow-on = 20; Resistance = 10</t>
+  </si>
+  <si>
+    <t>KRAS and NRAS  WT,
+HER2+</t>
+  </si>
+  <si>
+    <t>DNA/NGS-based detection,
+DNA/NGS-based detection or IHC or ISH</t>
+  </si>
+  <si>
+    <t>Olutasidenib</t>
+  </si>
+  <si>
+    <t>Mirvetuximab soravtansine</t>
+  </si>
+  <si>
+    <t>Quizartinib</t>
+  </si>
+  <si>
+    <t>Sacituzumab govitecan</t>
+  </si>
+  <si>
+    <t>Elacestrant</t>
+  </si>
+  <si>
+    <t>HR+/HER2-</t>
+  </si>
+  <si>
+    <t>FLT3
+ITD</t>
+  </si>
+  <si>
+    <t>FRɑ</t>
+  </si>
+  <si>
+    <t>IDH1
+R132C/G/H/L/S</t>
+  </si>
+  <si>
+    <t>IHC or IHC + ISH</t>
+  </si>
+  <si>
+    <t>DNA/NGS-based detection, 
+IHC</t>
+  </si>
+  <si>
+    <t>FGFR1 Fusions</t>
+  </si>
+  <si>
+    <t>NGS, Next-generation sequencing; ER, Estrogen Receptor; HR, Hormone Receptor; MSI-H, Microsatellite instability-high; TMB-H, Tumor mutational burden-high; dMMR, mismatch repair deficient; pMMR, mismatch repair proficient; PMSA, prostate-specific membrane antigen; FR, Folate Receptor; ITD, Internal Tandem Duplication</t>
+  </si>
+  <si>
+    <t>ESR1
+Ligand-binding domain missense mutations and
+ER+/HER2-</t>
+  </si>
+  <si>
+    <t>BCR-ABL1 Fusion
+and
+ABL1 T315I</t>
+  </si>
+  <si>
+    <t>KRAS and NRAS  Wildtype, and
+HER2+</t>
+  </si>
+  <si>
+    <t>ATM, ATR, BRCA1/2, CDK12, CHEK2, FANCA, MLH1, MRE11, NBN, PALB2, RAD51C
+Oncogenic Mutations</t>
+  </si>
+  <si>
+    <t>ATM, BARD1, BRCA1/2, BRIP1, CDK12, CHEK1/2, FANCL, PALB2, RAD51B, RAD51C, RAD51D, RAD54 Oncogenic Mutations</t>
+  </si>
+  <si>
+    <t>KRAS Wildtype and EGFR-expressing</t>
+  </si>
+  <si>
+    <t>EGFR L858R, Exon 19 Deletions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -609,6 +775,14 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -959,36 +1133,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2443C89-2C5B-8E41-851F-81266AC48571}">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1104,13 +1278,13 @@
         <v>117</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1301,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1155,7 +1329,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>14</v>
@@ -1178,7 +1352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2003</v>
       </c>
@@ -1186,7 +1360,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>138</v>
+        <v>199</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
@@ -1220,7 +1394,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>139</v>
+        <v>198</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>60</v>
@@ -1229,7 +1403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2004</v>
       </c>
@@ -1237,7 +1411,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>138</v>
+        <v>199</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>15</v>
@@ -1246,7 +1420,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2006</v>
       </c>
@@ -1257,7 +1431,7 @@
         <v>119</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>27</v>
@@ -1271,7 +1445,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>60</v>
@@ -1305,13 +1479,13 @@
         <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1331,7 +1505,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2009</v>
       </c>
@@ -1339,7 +1513,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>15</v>
@@ -1376,7 +1550,7 @@
         <v>120</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>14</v>
@@ -1407,7 +1581,7 @@
         <v>37</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>15</v>
@@ -1444,10 +1618,10 @@
         <v>18</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1464,7 +1638,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1475,13 +1649,13 @@
         <v>40</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1512,7 +1686,7 @@
         <v>18</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>3</v>
@@ -1526,13 +1700,13 @@
         <v>43</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1543,7 +1717,7 @@
         <v>44</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>15</v>
@@ -1577,7 +1751,7 @@
         <v>48</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>15</v>
@@ -1625,10 +1799,10 @@
         <v>2014</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>15</v>
@@ -1662,7 +1836,7 @@
         <v>55</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>15</v>
@@ -1671,7 +1845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2014</v>
       </c>
@@ -1679,7 +1853,7 @@
         <v>55</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>15</v>
@@ -1730,7 +1904,7 @@
         <v>56</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>6</v>
@@ -1753,7 +1927,7 @@
         <v>6</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -1764,30 +1938,30 @@
         <v>56</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>154</v>
+        <v>54</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>2015</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E48" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1795,16 +1969,16 @@
         <v>2015</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1812,16 +1986,16 @@
         <v>2015</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1832,10 +2006,10 @@
         <v>62</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>58</v>
+        <v>147</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>14</v>
@@ -1849,7 +2023,7 @@
         <v>62</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
@@ -1858,49 +2032,49 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2015</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2015</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>20</v>
+        <v>149</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>6</v>
@@ -1909,55 +2083,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>2016</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E56" s="2" t="s">
+      <c r="C57" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <v>2017</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>2017</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1965,27 +2139,27 @@
         <v>2017</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>2017</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>15</v>
@@ -1994,106 +2168,106 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>2017</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>18</v>
+        <v>151</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>2017</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>151</v>
+        <v>18</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>2017</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
-        <v>2018</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>2018</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>2018</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -2101,10 +2275,10 @@
         <v>2018</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>15</v>
@@ -2113,21 +2287,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>2018</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2135,10 +2309,10 @@
         <v>2018</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>15</v>
@@ -2152,16 +2326,16 @@
         <v>2018</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2169,61 +2343,61 @@
         <v>2018</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>2018</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E72" s="2" t="s">
+      <c r="C73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>15</v>
@@ -2232,21 +2406,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>2019</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2254,33 +2428,33 @@
         <v>2019</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>2019</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2288,36 +2462,36 @@
         <v>2019</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>2019</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>2019</v>
       </c>
@@ -2325,27 +2499,27 @@
         <v>87</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>167</v>
+        <v>18</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>15</v>
+        <v>179</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>14</v>
@@ -2353,30 +2527,30 @@
     </row>
     <row r="82" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>168</v>
+        <v>88</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>15</v>
@@ -2390,10 +2564,10 @@
         <v>2020</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>15</v>
@@ -2407,10 +2581,10 @@
         <v>2020</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>15</v>
@@ -2424,33 +2598,33 @@
         <v>2020</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>2020</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2458,33 +2632,33 @@
         <v>2020</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>2020</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>172</v>
+        <v>18</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2492,44 +2666,44 @@
         <v>2020</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>2020</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>2020</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>15</v>
@@ -2538,32 +2712,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>2020</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>2020</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>15</v>
@@ -2577,27 +2751,27 @@
         <v>2020</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>15</v>
@@ -2608,98 +2782,98 @@
     </row>
     <row r="97" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
         <v>2021</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B100" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E98" s="2" t="s">
+      <c r="C101" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A99" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B99" t="s">
-        <v>103</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D99" t="s">
-        <v>15</v>
-      </c>
-      <c r="E99" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B100" t="s">
-        <v>104</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D100" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B101" t="s">
-        <v>105</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D101" t="s">
-        <v>15</v>
-      </c>
-      <c r="E101" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>2021</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D102" t="s">
         <v>15</v>
@@ -2713,33 +2887,33 @@
         <v>2021</v>
       </c>
       <c r="B103" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>179</v>
+        <v>58</v>
       </c>
       <c r="D103" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E103" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>2021</v>
       </c>
       <c r="B104" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D104" t="s">
         <v>15</v>
       </c>
       <c r="E104" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2747,10 +2921,10 @@
         <v>2021</v>
       </c>
       <c r="B105" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>18</v>
+        <v>167</v>
       </c>
       <c r="D105" t="s">
         <v>15</v>
@@ -2761,62 +2935,194 @@
     </row>
     <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B106" t="s">
+        <v>107</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D106" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B107" t="s">
+        <v>108</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D107" t="s">
+        <v>15</v>
+      </c>
+      <c r="E107" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B108" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D108" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
         <v>2022</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B109" t="s">
         <v>110</v>
       </c>
-      <c r="C106" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D106" t="s">
-        <v>15</v>
-      </c>
-      <c r="E106" t="s">
+      <c r="C109" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D109" t="s">
+        <v>15</v>
+      </c>
+      <c r="E109" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="3">
+    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
         <v>2022</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B110" t="s">
         <v>111</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C110" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D110" t="s">
+        <v>171</v>
+      </c>
+      <c r="E110" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B111" t="s">
+        <v>112</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D111" t="s">
+        <v>172</v>
+      </c>
+      <c r="E111" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B112" t="s">
         <v>180</v>
       </c>
-      <c r="D107" t="s">
+      <c r="C112" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D112" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B113" t="s">
         <v>181</v>
       </c>
-      <c r="E107" t="s">
+      <c r="C113" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A108" s="3">
-        <v>2022</v>
-      </c>
-      <c r="B108" t="s">
-        <v>112</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D108" t="s">
+    <row r="114" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B114" t="s">
         <v>182</v>
       </c>
-      <c r="E108" t="s">
+      <c r="C114" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D114" t="s">
+        <v>15</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B115" t="s">
+        <v>183</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D115" t="s">
+        <v>189</v>
+      </c>
+      <c r="E115" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" spans="1:5" ht="67" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="31" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="204" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B116" t="s">
+        <v>184</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E116" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" spans="1:5" ht="204" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2829,7 +3135,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2837,9 +3143,9 @@
     <col min="1" max="1" width="116.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2848,7 +3154,7 @@
     </row>
     <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2857,7 +3163,7 @@
     </row>
     <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2866,7 +3172,7 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>130</v>
+        <v>174</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2875,7 +3181,7 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2884,16 +3190,16 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="238" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>135</v>
+        <v>176</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2902,7 +3208,7 @@
     </row>
     <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>133</v>
+        <v>192</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2911,7 +3217,7 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>134</v>
+        <v>177</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>

</xml_diff>